<commit_message>
Added superscript to CO2 and more tweaks and error checks
</commit_message>
<xml_diff>
--- a/data_cleaning/Assumptions_Insight_comments.xlsx
+++ b/data_cleaning/Assumptions_Insight_comments.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grahamke\Documents\GitHub\TIMES-NZ\TIMES_shiny\data_cleaning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grahamke\Documents\GitHub\TIMES-NZ\data_cleaning\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -98,9 +98,6 @@
     <t>Electricity Generation from Solar</t>
   </si>
   <si>
-    <t>Industrial emissions see a sharp decline in Kea to 2.7 Mt CO2/year in 2050 due to the uptake of direct use of renewables and electrification. Tūī declines more slowly as the transition takes longer.</t>
-  </si>
-  <si>
     <t>We estimated the number of new occupied dwellings under each scenario up to 2060 by dividing population increase projections by the number of new residents per new occupied dwelling, which was calculated from historical data.</t>
   </si>
   <si>
@@ -134,9 +131,6 @@
     <t>Kea’s more rapidly decreasing emissions indicate cumulative emissions through to 2050 being almost 25% lower in the Kea scenario than the Tūī scenario.</t>
   </si>
   <si>
-    <t>Both scenarios show strong reductions in energy emissions. Tūī declines to 10 Mt CO2/year in 2050 while Kea declines further to 6.5 Mt CO2/year.</t>
-  </si>
-  <si>
     <t>Both scenarios converge on a very high renewable electricity percentage of around 95%. Under both scenarios, winter gas peaking is retained, and there is a gradual decline in geothermal generation.  Under the Tūī scenario, hydro generation expands further, reducing dependence on gas peakers.</t>
   </si>
   <si>
@@ -171,6 +165,12 @@
   </si>
   <si>
     <t>Electrification across all sectors results in electricity demand roughly doubling in both scenarios, from 144 PJ in 2018 to around 280 PJ in 2060. Electricity supplies up to 59% in Kea and 57% in Tūī of all energy demand by 2060. Under both scenarios, this increased demand is met by very large increases in wind generation accompanied by large increases to solar (primarily grid-scale) in later years.</t>
+  </si>
+  <si>
+    <t>Both scenarios show strong reductions in energy emissions. Tūī declines to 10 Mt CO&lt;sup&gt;2&lt;/sup&gt;/year in 2050 while Kea declines further to 6.5 Mt CO&lt;sup&gt;2&lt;/sup&gt;/year.</t>
+  </si>
+  <si>
+    <t>Industrial emissions see a sharp decline in Kea to 2.7 Mt CO&lt;sup&gt;2&lt;/sup&gt;/year in 2050 due to the uptake of direct use of renewables and electrification. Tūī declines more slowly as the transition takes longer.</t>
   </si>
 </sst>
 </file>
@@ -491,7 +491,7 @@
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,7 +513,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -521,7 +521,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -537,31 +537,31 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -569,7 +569,7 @@
         <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -577,7 +577,7 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -585,7 +585,7 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -593,7 +593,7 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -601,7 +601,7 @@
         <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -609,7 +609,7 @@
         <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -617,7 +617,7 @@
         <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -625,7 +625,7 @@
         <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -633,7 +633,7 @@
         <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -641,7 +641,7 @@
         <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -649,7 +649,7 @@
         <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -657,7 +657,7 @@
         <v>22</v>
       </c>
       <c r="B20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -665,7 +665,7 @@
         <v>16</v>
       </c>
       <c r="B21" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -673,7 +673,7 @@
         <v>17</v>
       </c>
       <c r="B22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -681,7 +681,7 @@
         <v>18</v>
       </c>
       <c r="B23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -689,7 +689,7 @@
         <v>19</v>
       </c>
       <c r="B24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -697,7 +697,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>